<commit_message>
SmartContracts, Mist Notes and TimeRecordings.xlsx
</commit_message>
<xml_diff>
--- a/doc/Time_Recording.xlsx
+++ b/doc/Time_Recording.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Time Recording" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
   <si>
     <t xml:space="preserve">Time Recording</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve">Setting up a GIT Repo (Bitbucket, and finally GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting up Truffle (for developping smart contract) + Mist browser + dependencies (NPM, NodeJS, Electron, Gulp)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploying contract remotely &amp; locally + geth on 3 nodes</t>
   </si>
   <si>
     <t xml:space="preserve">Administration</t>
@@ -140,7 +146,7 @@
     <numFmt numFmtId="168" formatCode="[H]:MM"/>
     <numFmt numFmtId="169" formatCode="H:MM"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,12 +199,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -328,7 +328,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,14 +433,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,7 +489,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,16 +580,17 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="47.3481781376518"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -638,7 +631,7 @@
       </c>
       <c r="B4" s="11" t="n">
         <f aca="false">SUM(D7:D92)</f>
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
@@ -921,7 +914,7 @@
       <c r="E16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="24" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="25" t="s">
@@ -1052,7 +1045,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="n">
+      <c r="A22" s="26" t="n">
         <v>42660</v>
       </c>
       <c r="B22" s="22" t="n">
@@ -1200,35 +1193,55 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="n">
         <f aca="false">DATE(YEAR(A27),MONTH(A27),DAY(A27)+1)</f>
         <v>42663</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="22" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="C28" s="22" t="n">
+        <v>0.520833333333333</v>
+      </c>
       <c r="D28" s="18" t="n">
         <f aca="false">C28-B28</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0833333333333334</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="n">
         <f aca="false">DATE(YEAR(A28),MONTH(A28),DAY(A28)+1)</f>
         <v>42664</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="22" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="C29" s="22" t="n">
+        <v>0.729166666666667</v>
+      </c>
       <c r="D29" s="18" t="n">
         <f aca="false">C29-B29</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="n">
@@ -1261,7 +1274,7 @@
       <c r="G31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="18" t="n">
@@ -1273,7 +1286,7 @@
       <c r="G32" s="25"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="18" t="n">
@@ -1285,7 +1298,7 @@
       <c r="G33" s="25"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="28"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="18" t="n">
@@ -1297,7 +1310,7 @@
       <c r="G34" s="25"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="18" t="n">
@@ -1309,7 +1322,7 @@
       <c r="G35" s="25"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="28"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="18" t="n">
@@ -1321,7 +1334,7 @@
       <c r="G36" s="25"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="18" t="n">
@@ -1333,7 +1346,7 @@
       <c r="G37" s="25"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="28"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="18" t="n">
@@ -1345,7 +1358,7 @@
       <c r="G38" s="25"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="28"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="18" t="n">
@@ -1357,7 +1370,7 @@
       <c r="G39" s="25"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="28"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="18" t="n">
@@ -1369,7 +1382,7 @@
       <c r="G40" s="25"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="18" t="n">
@@ -1381,7 +1394,7 @@
       <c r="G41" s="25"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="18" t="n">
@@ -1393,7 +1406,7 @@
       <c r="G42" s="25"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="28"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="18" t="n">
@@ -1405,7 +1418,7 @@
       <c r="G43" s="25"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="28"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="18" t="n">
@@ -1417,7 +1430,7 @@
       <c r="G44" s="25"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="28"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="18" t="n">
@@ -1429,7 +1442,7 @@
       <c r="G45" s="25"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="28"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="18" t="n">
@@ -1441,7 +1454,7 @@
       <c r="G46" s="25"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="28"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="18" t="n">
@@ -1453,7 +1466,7 @@
       <c r="G47" s="25"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="28"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="18" t="n">
@@ -1465,7 +1478,7 @@
       <c r="G48" s="25"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="28"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="18" t="n">
@@ -1477,7 +1490,7 @@
       <c r="G49" s="25"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="28"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="18" t="n">
@@ -1489,7 +1502,7 @@
       <c r="G50" s="25"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="28"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="18" t="n">
@@ -1501,7 +1514,7 @@
       <c r="G51" s="25"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="28"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="18" t="n">
@@ -1513,7 +1526,7 @@
       <c r="G52" s="25"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="28"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
       <c r="D53" s="18" t="n">
@@ -1525,7 +1538,7 @@
       <c r="G53" s="25"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="28"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="18" t="n">
@@ -1537,7 +1550,7 @@
       <c r="G54" s="23"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="28"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="18" t="n">
@@ -1549,7 +1562,7 @@
       <c r="G55" s="23"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="28"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="18" t="n">
@@ -1561,7 +1574,7 @@
       <c r="G56" s="23"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="28"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
       <c r="D57" s="18" t="n">
@@ -1573,7 +1586,7 @@
       <c r="G57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="28"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="18" t="n">
@@ -1585,7 +1598,7 @@
       <c r="G58" s="25"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="28"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="18" t="n">
@@ -1597,7 +1610,7 @@
       <c r="G59" s="23"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="28"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
       <c r="D60" s="18" t="n">
@@ -1609,7 +1622,7 @@
       <c r="G60" s="23"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="28"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
       <c r="D61" s="18" t="n">
@@ -1621,7 +1634,7 @@
       <c r="G61" s="25"/>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="28"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="18" t="n">
@@ -1633,7 +1646,7 @@
       <c r="G62" s="25"/>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="28"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
       <c r="D63" s="18" t="n">
@@ -1645,7 +1658,7 @@
       <c r="G63" s="25"/>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="28"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
       <c r="D64" s="18" t="n">
@@ -1657,7 +1670,7 @@
       <c r="G64" s="25"/>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="28"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="22"/>
       <c r="C65" s="22"/>
       <c r="D65" s="18" t="n">
@@ -1669,7 +1682,7 @@
       <c r="G65" s="25"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="28"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
       <c r="D66" s="18" t="n">
@@ -1681,7 +1694,7 @@
       <c r="G66" s="25"/>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="28"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
       <c r="D67" s="18" t="n">
@@ -1693,7 +1706,7 @@
       <c r="G67" s="25"/>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="28"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
       <c r="D68" s="18" t="n">
@@ -1705,7 +1718,7 @@
       <c r="G68" s="25"/>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="28"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
       <c r="D69" s="18" t="n">
@@ -1717,7 +1730,7 @@
       <c r="G69" s="25"/>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="28"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
       <c r="D70" s="18" t="n">
@@ -1729,7 +1742,7 @@
       <c r="G70" s="25"/>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="28"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
       <c r="D71" s="18" t="n">
@@ -1741,7 +1754,7 @@
       <c r="G71" s="25"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="28"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="18" t="n">
@@ -1753,7 +1766,7 @@
       <c r="G72" s="25"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="28"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="18" t="n">
@@ -1765,7 +1778,7 @@
       <c r="G73" s="25"/>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="28"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="18" t="n">
@@ -1777,7 +1790,7 @@
       <c r="G74" s="25"/>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="28"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
       <c r="D75" s="18" t="n">
@@ -1789,7 +1802,7 @@
       <c r="G75" s="25"/>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="28"/>
+      <c r="A76" s="26"/>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
       <c r="D76" s="18" t="n">
@@ -1801,7 +1814,7 @@
       <c r="G76" s="25"/>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="28"/>
+      <c r="A77" s="26"/>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="18" t="n">
@@ -1813,7 +1826,7 @@
       <c r="G77" s="25"/>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="28"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
       <c r="D78" s="18" t="n">
@@ -1825,7 +1838,7 @@
       <c r="G78" s="25"/>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="28"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
       <c r="D79" s="18" t="n">
@@ -1837,7 +1850,7 @@
       <c r="G79" s="25"/>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="28"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
       <c r="D80" s="18" t="n">
@@ -1849,7 +1862,7 @@
       <c r="G80" s="25"/>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="28"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
       <c r="D81" s="18" t="n">
@@ -1861,7 +1874,7 @@
       <c r="G81" s="25"/>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="28"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
       <c r="D82" s="18" t="n">
@@ -1873,7 +1886,7 @@
       <c r="G82" s="25"/>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="28"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
       <c r="D83" s="18" t="n">
@@ -1885,7 +1898,7 @@
       <c r="G83" s="25"/>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="28"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="22"/>
       <c r="C84" s="22"/>
       <c r="D84" s="18" t="n">
@@ -1897,7 +1910,7 @@
       <c r="G84" s="25"/>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="28"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
       <c r="D85" s="18" t="n">
@@ -1909,7 +1922,7 @@
       <c r="G85" s="25"/>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="28"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
       <c r="D86" s="18" t="n">
@@ -1921,7 +1934,7 @@
       <c r="G86" s="25"/>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="28"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
       <c r="D87" s="18" t="n">
@@ -1933,7 +1946,7 @@
       <c r="G87" s="25"/>
     </row>
     <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="28"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
       <c r="D88" s="18" t="n">
@@ -1945,7 +1958,7 @@
       <c r="G88" s="25"/>
     </row>
     <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="28"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
       <c r="D89" s="18" t="n">
@@ -1957,7 +1970,7 @@
       <c r="G89" s="25"/>
     </row>
     <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="28"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
       <c r="D90" s="18" t="n">
@@ -1969,7 +1982,7 @@
       <c r="G90" s="25"/>
     </row>
     <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="28"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
       <c r="D91" s="18" t="n">
@@ -1981,30 +1994,30 @@
       <c r="G91" s="25"/>
     </row>
     <row r="92" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="29"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
+      <c r="A92" s="27"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="28"/>
       <c r="D92" s="18" t="n">
         <f aca="false">C92-B92</f>
         <v>0</v>
       </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="33"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="31"/>
     </row>
     <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="34"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="36" t="s">
+      <c r="A93" s="32"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D93" s="37" t="n">
+      <c r="D93" s="35" t="n">
         <f aca="false">SUM(D7:D92)</f>
-        <v>3.75</v>
-      </c>
-      <c r="E93" s="38"/>
-      <c r="F93" s="39"/>
-      <c r="G93" s="40"/>
+        <v>4</v>
+      </c>
+      <c r="E93" s="36"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2034,54 +2047,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.2834008097166"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="39" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="42" t="s">
-        <v>29</v>
+      <c r="B6" s="40" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="42" t="s">
-        <v>30</v>
+      <c r="B7" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="42" t="s">
-        <v>31</v>
+      <c r="B9" s="40" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="43" t="s">
-        <v>32</v>
+      <c r="B10" s="41" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="42" t="s">
-        <v>33</v>
+      <c r="B11" s="40" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="42" t="s">
-        <v>34</v>
+      <c r="B13" s="40" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various updates: papers,latex,time recordings
</commit_message>
<xml_diff>
--- a/doc/Time_Recording.xlsx
+++ b/doc/Time_Recording.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Time Recording" sheetId="1" state="visible" r:id="rId2"/>
@@ -152,13 +152,12 @@
     <numFmt numFmtId="168" formatCode="[H]:MM"/>
     <numFmt numFmtId="169" formatCode="H:MM"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,7 +180,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -189,7 +187,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -197,18 +194,10 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -217,7 +206,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -340,7 +328,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,14 +437,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,7 +489,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -598,19 +578,19 @@
   <dimension ref="1:96"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="59.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -624,7 +604,7 @@
       <c r="F1" s="0"/>
       <c r="G1" s="7" t="n">
         <f aca="true">TODAY()</f>
-        <v>42667</v>
+        <v>42695</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,7 +734,7 @@
       </c>
       <c r="D9" s="18" t="n">
         <f aca="false">C9-B9</f>
-        <v>0.083333333333333</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>9</v>
@@ -829,7 +809,7 @@
       </c>
       <c r="D12" s="18" t="n">
         <f aca="false">C12-B12</f>
-        <v>0.0416666666666666</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>14</v>
@@ -1039,7 +1019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="26" t="n">
         <f aca="false">DATE(YEAR(A19),MONTH(A19),DAY(A19)+3)</f>
         <v>42660</v>
@@ -1052,7 +1032,7 @@
       </c>
       <c r="D21" s="18" t="n">
         <f aca="false">C21-B21</f>
-        <v>0.0416666666666666</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>14</v>
@@ -1076,7 +1056,7 @@
       </c>
       <c r="D22" s="18" t="n">
         <f aca="false">C22-B22</f>
-        <v>0.0625000000000001</v>
+        <v>0.0625</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>16</v>
@@ -1226,7 +1206,7 @@
       </c>
       <c r="D28" s="18" t="n">
         <f aca="false">C28-B28</f>
-        <v>0.0833333333333334</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>16</v>
@@ -1264,7 +1244,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27" t="n">
+      <c r="A30" s="26" t="n">
         <v>42667</v>
       </c>
       <c r="B30" s="22" t="n">
@@ -1288,7 +1268,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="46.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="n">
+      <c r="A31" s="26" t="n">
         <v>42667</v>
       </c>
       <c r="B31" s="22" t="n">
@@ -1299,12 +1279,12 @@
       </c>
       <c r="D31" s="18" t="n">
         <f aca="false">C31-B31</f>
-        <v>0.0416666666666666</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="28" t="s">
+      <c r="F31" s="24" t="s">
         <v>32</v>
       </c>
       <c r="G31" s="25" t="s">
@@ -1312,7 +1292,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="27" t="n">
+      <c r="A32" s="26" t="n">
         <v>42667</v>
       </c>
       <c r="B32" s="22" t="n">
@@ -1323,7 +1303,7 @@
       </c>
       <c r="D32" s="18" t="n">
         <f aca="false">C32-B32</f>
-        <v>0.0625000000000001</v>
+        <v>0.0625</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>16</v>
@@ -1336,7 +1316,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="27" t="n">
+      <c r="A33" s="26" t="n">
         <v>42667</v>
       </c>
       <c r="B33" s="22" t="n">
@@ -2095,30 +2075,30 @@
       <c r="G94" s="25"/>
     </row>
     <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="29"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="28"/>
+      <c r="C95" s="28"/>
       <c r="D95" s="18" t="n">
         <f aca="false">C95-B95</f>
         <v>0</v>
       </c>
-      <c r="E95" s="31"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="33"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="30"/>
+      <c r="G95" s="31"/>
     </row>
     <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="34"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="36" t="s">
+      <c r="A96" s="32"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D96" s="37" t="n">
+      <c r="D96" s="35" t="n">
         <f aca="false">SUM(D7:D95)</f>
         <v>4.27083333333333</v>
       </c>
-      <c r="E96" s="38"/>
-      <c r="F96" s="39"/>
-      <c r="G96" s="40"/>
+      <c r="E96" s="36"/>
+      <c r="F96" s="37"/>
+      <c r="G96" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2148,53 +2128,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="39" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>